<commit_message>
fatto dei cambiamenti al frontend in base all'html fornito dal prof: - aggiunto bottoni per la scelta del modello - aggiunto delle hint visuali per far capire quali   feature sono obbligatori e quali no
TODO:
validazione degli input, gestione degli errori e
collegamento al backend.
</commit_message>
<xml_diff>
--- a/sito/diagnosi.xlsx
+++ b/sito/diagnosi.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -891,6 +891,38 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-04-23T09:15:35.407Z</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>149.132.61.23</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Likely NOT Malignant</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiunto la funzionalità di commit tramite backend
</commit_message>
<xml_diff>
--- a/sito/diagnosi.xlsx
+++ b/sito/diagnosi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -923,6 +923,102 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-05T14:57:30.993Z</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>149.132.26.74</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>uncertain case</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-07T16:19:03.014Z</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>93.66.5.34</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Likely NOT Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-05-07T16:22:36.511Z</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>93.66.5.34</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Likely Malignant</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
aggiustato problema dopo merge
</commit_message>
<xml_diff>
--- a/sito/diagnosi.xlsx
+++ b/sito/diagnosi.xlsx
@@ -425,13 +425,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="26" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="22" customWidth="1" min="8" max="8"/>
+    <col width="21" customWidth="1" min="9" max="9"/>
+    <col width="13" customWidth="1" min="10" max="10"/>
+    <col width="7" customWidth="1" min="11" max="11"/>
+    <col width="17" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="13" max="13"/>
+    <col width="5" customWidth="1" min="14" max="14"/>
+    <col width="5" customWidth="1" min="15" max="15"/>
+    <col width="9" customWidth="1" min="16" max="16"/>
+    <col width="9" customWidth="1" min="17" max="17"/>
+    <col width="13" customWidth="1" min="18" max="18"/>
+    <col width="15" customWidth="1" min="19" max="19"/>
+    <col width="21" customWidth="1" min="20" max="20"/>
+    <col width="13" customWidth="1" min="21" max="21"/>
+    <col width="13" customWidth="1" min="22" max="22"/>
+    <col width="14" customWidth="1" min="23" max="23"/>
+    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="18" customWidth="1" min="25" max="25"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -474,6 +501,91 @@
           <t>prediction</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Datetime</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Ip Address</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Hospital Center</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Protocol Code</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Max Dim</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Min Dim</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Veinous Inf</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Arterious Inf</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Duct Ret/Ductal Inv</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Vessel Comp</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Reg Margins</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Echogenicity</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Mult Lesions</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Prediction</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1016,6 +1128,104 @@
       <c r="H18" t="inlineStr">
         <is>
           <t>Likely Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2025-05-13 16:28:54</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>93.66.99.95</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" t="n">
+        <v>0</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>22.95% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2025-05-13 16:29:49</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>93.66.99.95</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>22.95% Malignant</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
aggiunto il DT calibrato
</commit_message>
<xml_diff>
--- a/sito/diagnosi.xlsx
+++ b/sito/diagnosi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1581,6 +1581,790 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:35:18</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>14% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:50:34</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
+        <v>0</v>
+      </c>
+      <c r="U29" t="n">
+        <v>0</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0</v>
+      </c>
+      <c r="X29" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>24% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:53:19</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>24% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:53:30</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>1</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" t="n">
+        <v>1</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>100% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:53:47</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>1</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0</v>
+      </c>
+      <c r="V32" t="n">
+        <v>1</v>
+      </c>
+      <c r="W32" t="n">
+        <v>1</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>100% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:57:28</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>24% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:57:40</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" t="n">
+        <v>1</v>
+      </c>
+      <c r="U34" t="n">
+        <v>1</v>
+      </c>
+      <c r="V34" t="n">
+        <v>1</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>67% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="E35" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:57:52</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>1</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>1</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>100% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:58:18</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" t="n">
+        <v>1</v>
+      </c>
+      <c r="W36" t="n">
+        <v>1</v>
+      </c>
+      <c r="X36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>29% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:58:28</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" t="n">
+        <v>0</v>
+      </c>
+      <c r="U37" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" t="n">
+        <v>0</v>
+      </c>
+      <c r="W37" t="n">
+        <v>1</v>
+      </c>
+      <c r="X37" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>0% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:58:37</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>1</v>
+      </c>
+      <c r="U38" t="n">
+        <v>1</v>
+      </c>
+      <c r="V38" t="n">
+        <v>0</v>
+      </c>
+      <c r="W38" t="n">
+        <v>0</v>
+      </c>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>84% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:58:55</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="R39" t="n">
+        <v>0</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>1</v>
+      </c>
+      <c r="U39" t="n">
+        <v>1</v>
+      </c>
+      <c r="V39" t="n">
+        <v>1</v>
+      </c>
+      <c r="W39" t="n">
+        <v>0</v>
+      </c>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>67% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:59:06</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0</v>
+      </c>
+      <c r="T40" t="n">
+        <v>1</v>
+      </c>
+      <c r="U40" t="n">
+        <v>1</v>
+      </c>
+      <c r="V40" t="n">
+        <v>1</v>
+      </c>
+      <c r="W40" t="n">
+        <v>0</v>
+      </c>
+      <c r="X40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="inlineStr">
+        <is>
+          <t>50% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" t="n">
+        <v>1</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:59:17</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0</v>
+      </c>
+      <c r="T41" t="n">
+        <v>1</v>
+      </c>
+      <c r="U41" t="n">
+        <v>1</v>
+      </c>
+      <c r="V41" t="n">
+        <v>1</v>
+      </c>
+      <c r="W41" t="n">
+        <v>0</v>
+      </c>
+      <c r="X41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>67% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:59:27</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0</v>
+      </c>
+      <c r="T42" t="n">
+        <v>1</v>
+      </c>
+      <c r="U42" t="n">
+        <v>1</v>
+      </c>
+      <c r="V42" t="n">
+        <v>1</v>
+      </c>
+      <c r="W42" t="n">
+        <v>1</v>
+      </c>
+      <c r="X42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>100% Malignant</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="E43" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2025-05-19 17:59:39</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>149.132.26.73</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>DT</t>
+        </is>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0</v>
+      </c>
+      <c r="S43" t="n">
+        <v>0</v>
+      </c>
+      <c r="T43" t="n">
+        <v>1</v>
+      </c>
+      <c r="U43" t="n">
+        <v>1</v>
+      </c>
+      <c r="V43" t="n">
+        <v>0</v>
+      </c>
+      <c r="W43" t="n">
+        <v>1</v>
+      </c>
+      <c r="X43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y43" t="inlineStr">
+        <is>
+          <t>75% Malignant</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>